<commit_message>
Update to ~190 citations
</commit_message>
<xml_diff>
--- a/ProcessedData/WOS_SciConf_20180531 (R1).xlsx
+++ b/ProcessedData/WOS_SciConf_20180531 (R1).xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\adit\My Documents\RG Citations\rgciting\ProcessedData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{F63847D3-8279-4282-B7BF-746A3A4547E1}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E9A7AA16-AD00-4765-9D1E-507699A9236B}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="9600" windowHeight="3312" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11238" uniqueCount="1415">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11238" uniqueCount="1425">
   <si>
     <t>AID</t>
   </si>
@@ -4266,6 +4266,36 @@
   </si>
   <si>
     <t>10.1145/2207676.2208640</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> IEEE 19th International Symposium on Personal, Indoor and Mobile Radio Communications</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.2527/jas2000.77E-Suppl1x</t>
+  </si>
+  <si>
+    <t>Journal of Animal Science</t>
+  </si>
+  <si>
+    <t>4 Season Company</t>
+  </si>
+  <si>
+    <t>https://www.fourseasonco.com.au/item/assessment-of-trace-mineral-status-of-ruminants-a-review</t>
+  </si>
+  <si>
+    <t>Proceedings of the 6th International ICST Conference on Simulation Tools and Techniques</t>
+  </si>
+  <si>
+    <t>https://dl.acm.org/citation.cfm?id=2512780; https://pdfs.semanticscholar.org/b1ab/b4bae8abf589e25a72a486d84a60f587d6df.pdf</t>
+  </si>
+  <si>
+    <t>10.4108/simutools.2013.251722</t>
+  </si>
+  <si>
+    <t>Annual Meeting of the Peripheral-Nerve-Society</t>
+  </si>
+  <si>
+    <t>https://onlinelibrary.wiley.com/toc/15298027/2007/12/s1</t>
   </si>
 </sst>
 </file>
@@ -5141,8 +5171,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AL332"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C130" workbookViewId="0">
-      <selection activeCell="V147" sqref="V147"/>
+    <sheetView tabSelected="1" topLeftCell="A140" workbookViewId="0">
+      <selection activeCell="T152" sqref="T152"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5151,7 +5181,7 @@
     <col min="18" max="18" width="19.21875" customWidth="1"/>
     <col min="20" max="20" width="2.5546875" customWidth="1"/>
     <col min="21" max="21" width="8.88671875" hidden="1" customWidth="1"/>
-    <col min="22" max="22" width="22.33203125" customWidth="1"/>
+    <col min="22" max="22" width="31.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:38" x14ac:dyDescent="0.3">
@@ -22092,37 +22122,37 @@
         <v>724</v>
       </c>
       <c r="C147" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="D147" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="E147" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="F147" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="G147" t="s">
-        <v>45</v>
+        <v>1415</v>
       </c>
       <c r="H147" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="I147" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="J147" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="K147" t="s">
-        <v>45</v>
-      </c>
-      <c r="L147" t="s">
-        <v>45</v>
+        <v>39</v>
+      </c>
+      <c r="L147" s="3" t="s">
+        <v>39</v>
       </c>
       <c r="M147" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="N147" t="s">
         <v>45</v>
@@ -22208,46 +22238,46 @@
         <v>727</v>
       </c>
       <c r="C148" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="D148" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="E148" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="F148" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="G148" t="s">
-        <v>45</v>
+        <v>1417</v>
       </c>
       <c r="H148" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="I148" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="J148" t="s">
-        <v>45</v>
+        <v>1418</v>
       </c>
       <c r="K148" t="s">
-        <v>45</v>
-      </c>
-      <c r="L148" t="s">
-        <v>45</v>
+        <v>1419</v>
+      </c>
+      <c r="L148" s="3" t="s">
+        <v>1416</v>
       </c>
       <c r="M148" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="N148" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="O148" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="P148" t="s">
-        <v>45</v>
+        <v>457</v>
       </c>
       <c r="Q148" t="s">
         <v>43</v>
@@ -22324,34 +22354,34 @@
         <v>730</v>
       </c>
       <c r="C149" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="D149" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="E149" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="F149" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="G149" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="H149" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="I149" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="J149" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="K149" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="L149" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="M149" t="s">
         <v>45</v>
@@ -22440,43 +22470,43 @@
         <v>733</v>
       </c>
       <c r="C150" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="D150" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="E150" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="F150" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="G150" t="s">
-        <v>45</v>
+        <v>1420</v>
       </c>
       <c r="H150" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="I150" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="J150" t="s">
-        <v>45</v>
+        <v>308</v>
       </c>
       <c r="K150" t="s">
-        <v>45</v>
+        <v>1421</v>
       </c>
       <c r="L150" t="s">
-        <v>45</v>
+        <v>1422</v>
       </c>
       <c r="M150" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="N150" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="O150" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="P150" t="s">
         <v>45</v>
@@ -22556,37 +22586,37 @@
         <v>736</v>
       </c>
       <c r="C151" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="D151" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="E151" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="F151" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="G151" t="s">
-        <v>45</v>
+        <v>1423</v>
       </c>
       <c r="H151" t="s">
         <v>45</v>
       </c>
       <c r="I151" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="J151" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="K151" t="s">
-        <v>45</v>
+        <v>1424</v>
       </c>
       <c r="L151" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="M151" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="N151" t="s">
         <v>45</v>
@@ -43675,8 +43705,9 @@
     <hyperlink ref="G143" r:id="rId14" display="https://link.springer.com/conference/icics" xr:uid="{F5D73287-4F74-4427-A728-D890EDA6AF0B}"/>
     <hyperlink ref="G146" r:id="rId15" tooltip="Conference Website" display="http://chi2012.acm.org/" xr:uid="{5169A432-FD2D-43AE-859C-126F780D5CD0}"/>
     <hyperlink ref="L146" r:id="rId16" display="https://doi.org/10.1145/2207676.2208640" xr:uid="{DE29CB30-56F0-43C5-8F4A-0D224D920721}"/>
+    <hyperlink ref="L148" r:id="rId17" xr:uid="{745291EB-226E-4303-9C90-41302E3699D6}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId17"/>
+  <pageSetup orientation="portrait" r:id="rId18"/>
 </worksheet>
 </file>
</xml_diff>